<commit_message>
Added more data to subjective response curve file
</commit_message>
<xml_diff>
--- a/DataCollection/QuestionnaireData/SubjectiveResponseCurve.xlsx
+++ b/DataCollection/QuestionnaireData/SubjectiveResponseCurve.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e005b3f8b47b9365/Documents/UiO/Other_projects/KetamineProject/DataCollection/QuestionnaireData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e005b3f8b47b9365/Documents/GitHub/Ketamine-project/DataCollection/QuestionnaireData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="94" documentId="8_{B13BE54D-C880-4C0D-B363-C263B962B823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65EEE528-C2ED-470E-A9B3-B0254A6A2F6F}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{B13BE54D-C880-4C0D-B363-C263B962B823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD82F907-DA81-4387-9916-5C2DB68FAAD1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{96B23907-5142-440F-9716-B0F0039B8C3F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{96B23907-5142-440F-9716-B0F0039B8C3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Participant ID</t>
   </si>
@@ -48,6 +48,15 @@
   </si>
   <si>
     <t>Pilot</t>
+  </si>
+  <si>
+    <t>SD5007</t>
+  </si>
+  <si>
+    <t>SD5008</t>
+  </si>
+  <si>
+    <t>AVG</t>
   </si>
 </sst>
 </file>
@@ -256,9 +265,6 @@
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -334,22 +340,13 @@
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A0E3-4F42-9314-DE8E26781ECF}"/>
+              <c16:uniqueId val="{00000003-947A-4C62-B622-54A2ECC4B438}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -433,7 +430,253 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-A0E3-4F42-9314-DE8E26781ECF}"/>
+              <c16:uniqueId val="{00000004-947A-4C62-B622-54A2ECC4B438}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SD5007</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$E$2:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-947A-4C62-B622-54A2ECC4B438}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SD5008</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$F$2:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-947A-4C62-B622-54A2ECC4B438}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$G$2:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.282758620689648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.013793103448258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78.999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.482758620689623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.910344827586172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98.910344827586172</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91.882758620689629</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.331034482758611</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.33793103448275</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-947A-4C62-B622-54A2ECC4B438}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -911,9 +1154,6 @@
                 <c:pt idx="12">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1001,15 +1241,6 @@
                 <c:pt idx="10">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1113,6 +1344,288 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-5ADE-49E4-882A-256FFD4D26A3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SD5007</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$E$2:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>98</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-84A1-4959-9E00-3CAF5EF6DC73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SD5008</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$F$2:$F$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-84A1-4959-9E00-3CAF5EF6DC73}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$G$2:$G$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.282758620689648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.013793103448258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78.999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.482758620689623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.910344827586172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98.910344827586172</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91.882758620689629</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.331034482758611</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.33793103448275</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-84A1-4959-9E00-3CAF5EF6DC73}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2533,16 +3046,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>187325</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>115887</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>657225</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>187325</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>7937</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2624,16 +3137,16 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>174625</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>122237</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>14287</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>174625</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>7937</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2961,15 +3474,15 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="P22" sqref="P22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2982,10 +3495,17 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -2999,11 +3519,18 @@
       <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <f>AVERAGE(B2:F2)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -3017,11 +3544,18 @@
       <c r="D3" s="1">
         <v>32</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="1">
+        <v>36</v>
+      </c>
+      <c r="F3" s="1">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" ref="G3:G15" si="0">AVERAGE(B3:F3)</f>
+        <v>22.282758620689648</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -3035,11 +3569,18 @@
       <c r="D4" s="1">
         <v>65</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="E4" s="1">
+        <v>98</v>
+      </c>
+      <c r="F4" s="1">
+        <v>36</v>
+      </c>
+      <c r="G4" s="1">
+        <f t="shared" si="0"/>
+        <v>57.013793103448258</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>30</v>
       </c>
@@ -3053,11 +3594,18 @@
       <c r="D5" s="1">
         <v>90</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="E5" s="1">
+        <v>100</v>
+      </c>
+      <c r="F5" s="1">
+        <v>54</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="0"/>
+        <v>78.999999999999972</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>40</v>
       </c>
@@ -3071,11 +3619,18 @@
       <c r="D6" s="1">
         <v>98</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="E6" s="1">
+        <v>100</v>
+      </c>
+      <c r="F6" s="1">
+        <v>68</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="0"/>
+        <v>82.482758620689623</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>50</v>
       </c>
@@ -3089,11 +3644,18 @@
       <c r="D7" s="1">
         <v>100</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="E7" s="1">
+        <v>100</v>
+      </c>
+      <c r="F7" s="1">
+        <v>83</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" si="0"/>
+        <v>93.910344827586172</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>60</v>
       </c>
@@ -3107,11 +3669,18 @@
       <c r="D8" s="1">
         <v>99</v>
       </c>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="E8" s="1">
+        <v>100</v>
+      </c>
+      <c r="F8" s="1">
+        <v>100</v>
+      </c>
+      <c r="G8" s="1">
+        <f t="shared" si="0"/>
+        <v>98.910344827586172</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>70</v>
       </c>
@@ -3125,11 +3694,18 @@
       <c r="D9" s="1">
         <v>95</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="E9" s="1">
+        <v>98</v>
+      </c>
+      <c r="F9" s="1">
+        <v>94</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="0"/>
+        <v>91.882758620689629</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>80</v>
       </c>
@@ -3143,11 +3719,18 @@
       <c r="D10" s="1">
         <v>92</v>
       </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="E10" s="1">
+        <v>93</v>
+      </c>
+      <c r="F10" s="1">
+        <v>67</v>
+      </c>
+      <c r="G10" s="1">
+        <f t="shared" si="0"/>
+        <v>78.331034482758611</v>
+      </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>90</v>
       </c>
@@ -3161,11 +3744,18 @@
       <c r="D11" s="1">
         <v>82</v>
       </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="E11" s="1">
+        <v>84</v>
+      </c>
+      <c r="F11" s="1">
+        <v>45</v>
+      </c>
+      <c r="G11" s="1">
+        <f t="shared" si="0"/>
+        <v>66.33793103448275</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>100</v>
       </c>
@@ -3178,104 +3768,117 @@
       <c r="D12" s="1">
         <v>66</v>
       </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="E12" s="1">
+        <v>68</v>
+      </c>
+      <c r="F12" s="1">
+        <v>12</v>
+      </c>
+      <c r="G12" s="1">
+        <f t="shared" si="0"/>
+        <v>44.2</v>
+      </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>110</v>
       </c>
       <c r="B13">
         <v>26</v>
       </c>
-      <c r="C13" s="1">
-        <v>0</v>
-      </c>
+      <c r="C13" s="1"/>
       <c r="D13" s="1">
         <v>51</v>
       </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="E13" s="1">
+        <v>52</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <f t="shared" si="0"/>
+        <v>32.25</v>
+      </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>120</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
-      <c r="C14" s="1">
-        <v>0</v>
-      </c>
+      <c r="C14" s="1"/>
       <c r="D14" s="1">
         <v>30</v>
       </c>
+      <c r="E14" s="1">
+        <v>33</v>
+      </c>
+      <c r="G14" s="1">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>130</v>
       </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>0</v>
-      </c>
+      <c r="C15" s="1"/>
       <c r="D15" s="1">
         <v>0</v>
       </c>
-      <c r="E15" s="1"/>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>140</v>
       </c>
-      <c r="B16">
-        <f>AVERAGE(B2:B15)</f>
-        <v>53.142857142857146</v>
-      </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>150</v>
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>160</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>170</v>
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>180</v>
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>190</v>
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SD5009 and SD5010 to distribution
</commit_message>
<xml_diff>
--- a/DataCollection/QuestionnaireData/SubjectiveResponseCurve.xlsx
+++ b/DataCollection/QuestionnaireData/SubjectiveResponseCurve.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e005b3f8b47b9365/Documents/GitHub/Ketamine-project/DataCollection/QuestionnaireData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\platon.uio.no\med-imb-u1\andrlm\pc\Dokumenter\GitHub\Ketamine-project\DataCollection\QuestionnaireData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{B13BE54D-C880-4C0D-B363-C263B962B823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AD82F907-DA81-4387-9916-5C2DB68FAAD1}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{96B23907-5142-440F-9716-B0F0039B8C3F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Participant ID</t>
   </si>
@@ -58,11 +57,17 @@
   <si>
     <t>AVG</t>
   </si>
+  <si>
+    <t>SD5009</t>
+  </si>
+  <si>
+    <t>SD5010</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -117,7 +122,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nb-NO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -149,7 +154,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="nb-NO"/>
-              <a:t>Subjectice response over</a:t>
+              <a:t>Subjective response over</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="nb-NO" baseline="0"/>
@@ -159,6 +164,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -601,7 +607,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Ark1'!$G$1</c:f>
+              <c:f>'Ark1'!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -624,7 +630,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$G$2:$G$15</c:f>
+              <c:f>'Ark1'!$I$2:$I$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -725,6 +731,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -844,6 +851,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -918,6 +926,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -949,6 +958,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -956,7 +966,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -994,7 +1003,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="nb-NO"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1012,7 +1021,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1036,6 +1045,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1049,7 +1059,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -1086,7 +1096,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -1095,8 +1105,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
@@ -1105,16 +1115,17 @@
                 <a:solidFill>
                   <a:schemeClr val="accent1"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$B$2:$B$15</c:f>
+              <c:f>'Ark1'!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1160,7 +1171,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5ADE-49E4-882A-256FFD4D26A3}"/>
+              <c16:uniqueId val="{00000000-E585-41FC-87B5-9E645A53313A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1179,7 +1190,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -1188,8 +1199,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="square"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
@@ -1198,16 +1209,17 @@
                 <a:solidFill>
                   <a:schemeClr val="accent2"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$C$2:$C$15</c:f>
+              <c:f>'Ark1'!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1247,7 +1259,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5ADE-49E4-882A-256FFD4D26A3}"/>
+              <c16:uniqueId val="{00000001-E585-41FC-87B5-9E645A53313A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1266,7 +1278,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -1275,8 +1287,8 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="triangle"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
@@ -1285,16 +1297,17 @@
                 <a:solidFill>
                   <a:schemeClr val="accent3"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$D$2:$D$15</c:f>
+              <c:f>'Ark1'!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1343,7 +1356,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5ADE-49E4-882A-256FFD4D26A3}"/>
+              <c16:uniqueId val="{00000002-E585-41FC-87B5-9E645A53313A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1362,7 +1375,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -1371,26 +1384,25 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent4"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$E$2:$E$15</c:f>
+              <c:f>'Ark1'!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1439,7 +1451,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-84A1-4959-9E00-3CAF5EF6DC73}"/>
+              <c16:uniqueId val="{00000003-E585-41FC-87B5-9E645A53313A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1458,7 +1470,7 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
@@ -1467,26 +1479,25 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="star"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent5"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:ln w="9525">
                 <a:solidFill>
                   <a:schemeClr val="accent5"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$F$2:$F$15</c:f>
+              <c:f>'Ark1'!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1529,7 +1540,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-84A1-4959-9E00-3CAF5EF6DC73}"/>
+              <c16:uniqueId val="{00000004-E585-41FC-87B5-9E645A53313A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1542,13 +1553,13 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>AVG</c:v>
+                  <c:v>SD5009</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
               </a:solidFill>
@@ -1558,7 +1569,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="6"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="accent6"/>
@@ -1567,56 +1578,36 @@
                 <a:solidFill>
                   <a:schemeClr val="accent6"/>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Ark1'!$G$2:$G$15</c:f>
+              <c:f>'Ark1'!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.282758620689648</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57.013793103448258</c:v>
+                  <c:v>92</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>78.999999999999972</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>82.482758620689623</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>93.910344827586172</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>98.910344827586172</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>91.882758620689629</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>78.331034482758611</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>66.33793103448275</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>44.2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>32.25</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="13">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -1625,7 +1616,198 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-84A1-4959-9E00-3CAF5EF6DC73}"/>
+              <c16:uniqueId val="{00000005-E585-41FC-87B5-9E645A53313A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SD5010</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="plus"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$H$2:$H$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-E585-41FC-87B5-9E645A53313A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Ark1'!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="dot"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Ark1'!$I$2:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.282758620689648</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.013793103448258</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>78.999999999999972</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>82.482758620689623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>93.910344827586172</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>98.910344827586172</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>91.882758620689629</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>78.331034482758611</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>66.33793103448275</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>44.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.25</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-E585-41FC-87B5-9E645A53313A}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1639,16 +1821,30 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="486814063"/>
-        <c:axId val="486807823"/>
+        <c:axId val="492362784"/>
+        <c:axId val="492360816"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="486814063"/>
+        <c:axId val="492362784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1656,7 +1852,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1675,6 +1871,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1688,7 +1885,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1704,7 +1901,6 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1713,6 +1909,113 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="nb-NO"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="492360816"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="492360816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="nb-NO"/>
+                  <a:t>Response</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nb-NO"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
                 <a:lumMod val="15000"/>
                 <a:lumOff val="85000"/>
               </a:schemeClr>
@@ -1741,122 +2044,7 @@
             <a:endParaRPr lang="nb-NO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="486807823"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="486807823"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="100"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="nb-NO"/>
-                  <a:t>Response</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="nb-NO"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="nb-NO"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="486814063"/>
+        <c:crossAx val="492362784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1869,7 +2057,8 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1901,18 +2090,11 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -2540,7 +2722,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2551,7 +2733,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -2574,18 +2756,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -2597,7 +2779,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -2605,11 +2787,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -2641,35 +2823,45 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -2681,30 +2873,34 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -2726,15 +2922,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -2749,15 +2943,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2768,17 +2962,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -2787,10 +2980,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -2806,21 +2999,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2839,17 +3026,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -2858,17 +3044,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -2877,17 +3062,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -2908,7 +3092,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -2916,7 +3100,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -2929,6 +3113,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -2936,10 +3131,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -2960,7 +3155,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -2969,14 +3164,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -2990,7 +3185,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -3006,8 +3201,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -3023,6 +3218,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -3030,14 +3236,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -3046,16 +3246,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>187325</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>115887</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>49212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>187325</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>131762</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3137,26 +3337,20 @@
   </xdr:oneCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>174625</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>122237</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>174625</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Diagram 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{997B5BE9-2F2A-82BE-42D4-882225BA5C1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3470,19 +3664,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B57709-2DDF-4FA7-AC01-A2FDC07F7C08}">
-  <dimension ref="A1:G23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3502,10 +3696,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3526,11 +3726,17 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1">
         <f>AVERAGE(B2:F2)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -3551,11 +3757,17 @@
         <v>16</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G15" si="0">AVERAGE(B3:F3)</f>
+        <v>100</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1">
+        <f>AVERAGE(B3:F3)</f>
         <v>22.282758620689648</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>20</v>
       </c>
@@ -3576,11 +3788,17 @@
         <v>36</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+      <c r="I4" s="1">
+        <f>AVERAGE(B4:F4)</f>
         <v>57.013793103448258</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>30</v>
       </c>
@@ -3601,11 +3819,17 @@
         <v>54</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="0"/>
+        <v>86</v>
+      </c>
+      <c r="H5" s="1">
+        <v>30</v>
+      </c>
+      <c r="I5" s="1">
+        <f>AVERAGE(B5:F5)</f>
         <v>78.999999999999972</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>40</v>
       </c>
@@ -3626,11 +3850,17 @@
         <v>68</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="0"/>
+        <v>84</v>
+      </c>
+      <c r="H6" s="1">
+        <v>74</v>
+      </c>
+      <c r="I6" s="1">
+        <f>AVERAGE(B6:F6)</f>
         <v>82.482758620689623</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>50</v>
       </c>
@@ -3651,11 +3881,17 @@
         <v>83</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H7" s="1">
+        <v>100</v>
+      </c>
+      <c r="I7" s="1">
+        <f>AVERAGE(B7:F7)</f>
         <v>93.910344827586172</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>60</v>
       </c>
@@ -3676,11 +3912,17 @@
         <v>100</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>94</v>
+      </c>
+      <c r="I8" s="1">
+        <f>AVERAGE(B8:F8)</f>
         <v>98.910344827586172</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>70</v>
       </c>
@@ -3700,12 +3942,15 @@
       <c r="F9" s="1">
         <v>94</v>
       </c>
-      <c r="G9" s="1">
-        <f t="shared" si="0"/>
+      <c r="H9" s="1">
+        <v>84</v>
+      </c>
+      <c r="I9" s="1">
+        <f>AVERAGE(B9:F9)</f>
         <v>91.882758620689629</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>80</v>
       </c>
@@ -3725,12 +3970,15 @@
       <c r="F10" s="1">
         <v>67</v>
       </c>
-      <c r="G10" s="1">
-        <f t="shared" si="0"/>
+      <c r="H10" s="1">
+        <v>66</v>
+      </c>
+      <c r="I10" s="1">
+        <f>AVERAGE(B10:F10)</f>
         <v>78.331034482758611</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>90</v>
       </c>
@@ -3750,12 +3998,15 @@
       <c r="F11" s="1">
         <v>45</v>
       </c>
-      <c r="G11" s="1">
-        <f t="shared" si="0"/>
+      <c r="H11" s="1">
+        <v>34</v>
+      </c>
+      <c r="I11" s="1">
+        <f>AVERAGE(B11:F11)</f>
         <v>66.33793103448275</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>100</v>
       </c>
@@ -3774,12 +4025,15 @@
       <c r="F12" s="1">
         <v>12</v>
       </c>
-      <c r="G12" s="1">
-        <f t="shared" si="0"/>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <f>AVERAGE(B12:F12)</f>
         <v>44.2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>110</v>
       </c>
@@ -3796,12 +4050,12 @@
       <c r="F13" s="1">
         <v>0</v>
       </c>
-      <c r="G13" s="1">
-        <f t="shared" si="0"/>
+      <c r="I13" s="1">
+        <f>AVERAGE(B13:F13)</f>
         <v>32.25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>120</v>
       </c>
@@ -3815,12 +4069,12 @@
       <c r="E14" s="1">
         <v>33</v>
       </c>
-      <c r="G14" s="1">
-        <f t="shared" si="0"/>
+      <c r="I14" s="1">
+        <f>AVERAGE(B14:F14)</f>
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>130</v>
       </c>
@@ -3832,53 +4086,53 @@
         <v>0</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="1">
-        <f t="shared" si="0"/>
+      <c r="I15" s="1">
+        <f>AVERAGE(B15:F15)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>140</v>
       </c>
       <c r="E16" s="1"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>150</v>
       </c>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>160</v>
       </c>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>170</v>
       </c>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>180</v>
       </c>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>190</v>
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>200</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
   </sheetData>

</xml_diff>